<commit_message>
New files; all web operations are functional now.
</commit_message>
<xml_diff>
--- a/source/Cash_Severna.xlsx
+++ b/source/Cash_Severna.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\filesrv\uf\kassir\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8795D81B-ABAC-45A6-9277-21DE43ED4FE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F31289-6B25-4CA0-B6A2-6083E87EC02C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -954,7 +954,7 @@
       <selection activeCell="BO16" sqref="BO16"/>
       <selection pane="topRight" activeCell="BO16" sqref="BO16"/>
       <selection pane="bottomLeft" activeCell="BO16" sqref="BO16"/>
-      <selection pane="bottomRight" activeCell="N39" sqref="N39"/>
+      <selection pane="bottomRight" activeCell="P39" sqref="P39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1164,8 +1164,12 @@
       <c r="N4" s="70">
         <v>454250018</v>
       </c>
-      <c r="O4" s="70"/>
-      <c r="P4" s="70"/>
+      <c r="O4" s="70">
+        <v>476239363</v>
+      </c>
+      <c r="P4" s="70">
+        <v>377198108</v>
+      </c>
       <c r="Q4" s="70"/>
       <c r="R4" s="70"/>
       <c r="S4" s="70"/>
@@ -1220,8 +1224,12 @@
       <c r="N5" s="70">
         <v>192729</v>
       </c>
-      <c r="O5" s="70"/>
-      <c r="P5" s="70"/>
+      <c r="O5" s="70">
+        <v>192729</v>
+      </c>
+      <c r="P5" s="70">
+        <v>192729</v>
+      </c>
       <c r="Q5" s="70"/>
       <c r="R5" s="70"/>
       <c r="S5" s="70"/>
@@ -1276,8 +1284,12 @@
       <c r="N6" s="70">
         <v>87328027</v>
       </c>
-      <c r="O6" s="70"/>
-      <c r="P6" s="70"/>
+      <c r="O6" s="70">
+        <v>134272848</v>
+      </c>
+      <c r="P6" s="70">
+        <v>130226460</v>
+      </c>
       <c r="Q6" s="70"/>
       <c r="R6" s="70"/>
       <c r="S6" s="70"/>
@@ -1332,8 +1344,12 @@
       <c r="N7" s="70">
         <v>6116154</v>
       </c>
-      <c r="O7" s="70"/>
-      <c r="P7" s="70"/>
+      <c r="O7" s="70">
+        <v>5400661</v>
+      </c>
+      <c r="P7" s="70">
+        <v>5400091</v>
+      </c>
       <c r="Q7" s="70"/>
       <c r="R7" s="70"/>
       <c r="S7" s="70"/>
@@ -1388,8 +1404,12 @@
       <c r="N8" s="70">
         <v>691903</v>
       </c>
-      <c r="O8" s="70"/>
-      <c r="P8" s="70"/>
+      <c r="O8" s="70">
+        <v>354691</v>
+      </c>
+      <c r="P8" s="70">
+        <v>1799479</v>
+      </c>
       <c r="Q8" s="70"/>
       <c r="R8" s="70"/>
       <c r="S8" s="70"/>
@@ -1444,8 +1464,12 @@
       <c r="N9" s="70">
         <v>12113755</v>
       </c>
-      <c r="O9" s="70"/>
-      <c r="P9" s="70"/>
+      <c r="O9" s="70">
+        <v>12112955</v>
+      </c>
+      <c r="P9" s="70">
+        <v>12109637</v>
+      </c>
       <c r="Q9" s="70"/>
       <c r="R9" s="70"/>
       <c r="S9" s="70"/>
@@ -1500,8 +1524,12 @@
       <c r="N10" s="70">
         <v>7610040</v>
       </c>
-      <c r="O10" s="70"/>
-      <c r="P10" s="70"/>
+      <c r="O10" s="70">
+        <v>7610040</v>
+      </c>
+      <c r="P10" s="70">
+        <v>7610040</v>
+      </c>
       <c r="Q10" s="70"/>
       <c r="R10" s="70"/>
       <c r="S10" s="70"/>
@@ -1554,8 +1582,12 @@
       <c r="N11" s="70">
         <v>118575</v>
       </c>
-      <c r="O11" s="70"/>
-      <c r="P11" s="70"/>
+      <c r="O11" s="70">
+        <v>118575</v>
+      </c>
+      <c r="P11" s="70">
+        <v>115075</v>
+      </c>
       <c r="Q11" s="70"/>
       <c r="R11" s="70"/>
       <c r="S11" s="70"/>
@@ -1944,8 +1976,12 @@
       <c r="N24" s="70">
         <v>1244543</v>
       </c>
-      <c r="O24" s="70"/>
-      <c r="P24" s="70"/>
+      <c r="O24" s="70">
+        <v>1244543</v>
+      </c>
+      <c r="P24" s="70">
+        <v>1244543</v>
+      </c>
       <c r="Q24" s="70"/>
       <c r="R24" s="70"/>
       <c r="S24" s="70"/>
@@ -2080,8 +2116,12 @@
       <c r="N27" s="70">
         <v>1688703</v>
       </c>
-      <c r="O27" s="70"/>
-      <c r="P27" s="70"/>
+      <c r="O27" s="70">
+        <v>1688703</v>
+      </c>
+      <c r="P27" s="70">
+        <v>1688703</v>
+      </c>
       <c r="Q27" s="70"/>
       <c r="R27" s="70"/>
       <c r="S27" s="70"/>
@@ -2226,8 +2266,12 @@
       <c r="N32" s="70">
         <v>45152761</v>
       </c>
-      <c r="O32" s="70"/>
-      <c r="P32" s="70"/>
+      <c r="O32" s="70">
+        <v>45152761</v>
+      </c>
+      <c r="P32" s="70">
+        <v>45112051</v>
+      </c>
       <c r="Q32" s="70"/>
       <c r="R32" s="70"/>
       <c r="S32" s="70"/>
@@ -2318,8 +2362,12 @@
       <c r="N34" s="70">
         <v>5240700</v>
       </c>
-      <c r="O34" s="70"/>
-      <c r="P34" s="70"/>
+      <c r="O34" s="70">
+        <v>5240700</v>
+      </c>
+      <c r="P34" s="70">
+        <v>5240700</v>
+      </c>
       <c r="Q34" s="70"/>
       <c r="R34" s="70"/>
       <c r="S34" s="70"/>
@@ -2410,8 +2458,12 @@
       <c r="N36" s="70">
         <v>1424705</v>
       </c>
-      <c r="O36" s="70"/>
-      <c r="P36" s="70"/>
+      <c r="O36" s="70">
+        <v>1424705</v>
+      </c>
+      <c r="P36" s="70">
+        <v>1424705</v>
+      </c>
       <c r="Q36" s="70"/>
       <c r="R36" s="70"/>
       <c r="S36" s="70"/>
@@ -2502,8 +2554,12 @@
       <c r="N38" s="70">
         <v>320000</v>
       </c>
-      <c r="O38" s="70"/>
-      <c r="P38" s="70"/>
+      <c r="O38" s="70">
+        <v>320000</v>
+      </c>
+      <c r="P38" s="70">
+        <v>320000</v>
+      </c>
       <c r="Q38" s="70"/>
       <c r="R38" s="70"/>
       <c r="S38" s="70"/>

</xml_diff>